<commit_message>
improve  report account transaction
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/account_trans.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/account_trans.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">{{#if track_name}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Tracking: {{track_name}}</t>
+    <t xml:space="preserve">Tracking-1: {{track_name}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{/if}}</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">{{#if track2_name}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Tracking: {{track2_name}}</t>
+    <t xml:space="preserve">Tracking-2: {{track2_name}}</t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Contact</t>
   </si>
   <si>
-    <t xml:space="preserve">Tracking</t>
+    <t xml:space="preserve">Tracking-1</t>
   </si>
   <si>
     <t xml:space="preserve">Tracking-2</t>
@@ -534,7 +534,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -542,14 +542,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>